<commit_message>
+ question3 with excel activities
</commit_message>
<xml_diff>
--- a/Data/Output/Question3.xlsx
+++ b/Data/Output/Question3.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Day_3\Data\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\Shireen_Day_3_last\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC4B26A-C21B-4555-B38F-AAED71958D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DA8B6C-68B3-45AA-ADBF-561BF2487C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sum" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="Sum" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Cash In</t>
   </si>
@@ -35,6 +36,15 @@
   </si>
   <si>
     <t>19565</t>
+  </si>
+  <si>
+    <t>CashIn</t>
+  </si>
+  <si>
+    <t>OnCheck</t>
+  </si>
+  <si>
+    <t>NotOnCheck</t>
   </si>
 </sst>
 </file>
@@ -372,16 +382,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B55BAE6-9928-4623-B4DF-C7A36891B030}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H45" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>35630</v>
+      </c>
+      <c r="B2">
+        <v>179809</v>
+      </c>
+      <c r="C2">
+        <v>19565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,7 +439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>